<commit_message>
Prepare app for Render deployment
</commit_message>
<xml_diff>
--- a/Gen_AI Dataset.xlsx
+++ b/Gen_AI Dataset.xlsx
@@ -568,7 +568,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,13 +586,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1052,155 +1045,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1543,11 +1539,11 @@
   <sheetPr/>
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="255" customWidth="1"/>
     <col min="2" max="2" width="122.625" customWidth="1"/>
@@ -1721,8 +1717,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="22" ht="409.5" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
@@ -1997,7 +1993,7 @@
       <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2121,7 +2117,7 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" ht="15" spans="1:1">
       <c r="A1" s="1" t="s">

</xml_diff>